<commit_message>
Edited jvm options for tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TESTY.xlsx
+++ b/src/main/resources/TESTY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romis\Desktop\fav\Bachelor_thesis_code\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romis\Documents\Bachelor_thesis_code\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105B7D3F-99B3-4038-8020-58540D357B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF981668-C1C0-4465-B2D0-AD3CE6C5BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{450F20DB-53D6-4CB5-91FD-25E685046F21}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="7" xr2:uid="{450F20DB-53D6-4CB5-91FD-25E685046F21}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="E" sheetId="7" r:id="rId5"/>
     <sheet name="F" sheetId="8" r:id="rId6"/>
     <sheet name="G" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="46">
   <si>
     <t>Link struktura</t>
   </si>
@@ -186,6 +187,30 @@
   <si>
     <t>Ignorování jednoduché [ms]</t>
   </si>
+  <si>
+    <t>Testy [Byte]</t>
+  </si>
+  <si>
+    <t>Kód [Byte]</t>
+  </si>
+  <si>
+    <t>Základní</t>
+  </si>
+  <si>
+    <t>Dědičnost</t>
+  </si>
+  <si>
+    <t>Ignorování</t>
+  </si>
+  <si>
+    <t>Kolekce a mapy</t>
+  </si>
+  <si>
+    <t>Speciální případy</t>
+  </si>
+  <si>
+    <t>Počet testů</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +326,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -656,11 +681,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,9 +952,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2509,7 +2597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2832,20 +2920,20 @@
       <selection activeCell="K15" sqref="K15:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="45"/>
     </row>
-    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
@@ -2889,7 +2977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -2934,7 +3022,7 @@
         <v>0.31240999999999997</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -2979,7 +3067,7 @@
         <v>2.0545</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -3024,7 +3112,7 @@
         <v>10.043800000000001</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -3069,7 +3157,7 @@
         <v>67.405900000000003</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -3114,8 +3202,8 @@
         <v>983.47350000000006</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K15" s="63" t="str">
         <f t="shared" ref="K15:K20" si="0">C5</f>
         <v>Šířka [-]</v>
@@ -3124,7 +3212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
       <c r="K16" s="61">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3134,7 +3222,7 @@
         <v>0.31240999999999997</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="K17" s="58">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -3144,7 +3232,7 @@
         <v>2.0545</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="K18" s="58">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -3154,7 +3242,7 @@
         <v>10.043800000000001</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="K19" s="58">
         <f t="shared" si="0"/>
         <v>100000</v>
@@ -3164,7 +3252,7 @@
         <v>67.405900000000003</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K20" s="53">
         <f t="shared" si="0"/>
         <v>1000000</v>
@@ -3174,7 +3262,7 @@
         <v>983.47350000000006</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" s="54"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
@@ -3182,7 +3270,7 @@
       <c r="G27" s="55"/>
       <c r="H27" s="55"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="54"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -3206,17 +3294,17 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3260,7 +3348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -3305,7 +3393,7 @@
         <v>0.20220000000000002</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -3350,7 +3438,7 @@
         <v>0.52510000000000001</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -3395,7 +3483,7 @@
         <v>3.4866000000000001</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -3440,7 +3528,7 @@
         <v>40.417499999999997</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -3485,8 +3573,8 @@
         <v>434.0449999999999</v>
       </c>
     </row>
-    <row r="24" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D25" s="63" t="s">
         <v>1</v>
       </c>
@@ -3494,7 +3582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D26" s="67">
         <f t="shared" ref="D26:D30" si="1">C6</f>
         <v>100</v>
@@ -3504,7 +3592,7 @@
         <v>0.20220000000000002</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D27" s="65">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -3514,7 +3602,7 @@
         <v>0.52510000000000001</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D28" s="65">
         <f t="shared" si="1"/>
         <v>10000</v>
@@ -3524,7 +3612,7 @@
         <v>3.4866000000000001</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D29" s="65">
         <f t="shared" si="1"/>
         <v>100000</v>
@@ -3534,7 +3622,7 @@
         <v>40.417499999999997</v>
       </c>
     </row>
-    <row r="30" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D30" s="66">
         <f t="shared" si="1"/>
         <v>1000000</v>
@@ -3556,26 +3644,26 @@
   <sheetPr codeName="List3"/>
   <dimension ref="B3:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3619,7 +3707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -3664,7 +3752,7 @@
         <v>4.8865999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>500</v>
       </c>
@@ -3709,7 +3797,7 @@
         <v>145.55210000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>1000</v>
       </c>
@@ -3754,7 +3842,7 @@
         <v>710.81810000000007</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>2000</v>
       </c>
@@ -3799,7 +3887,7 @@
         <v>2992.3115999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>5000</v>
       </c>
@@ -3844,8 +3932,8 @@
         <v>21777.465200000002</v>
       </c>
     </row>
-    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="63" t="s">
         <v>28</v>
       </c>
@@ -3853,7 +3941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="67">
         <f t="shared" ref="C29:C33" si="1">C6</f>
         <v>100</v>
@@ -3863,7 +3951,7 @@
         <v>4.8865999999999996</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="65">
         <f t="shared" si="1"/>
         <v>500</v>
@@ -3873,7 +3961,7 @@
         <v>145.55210000000002</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="65">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -3883,7 +3971,7 @@
         <v>710.81810000000007</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="65">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -3893,7 +3981,7 @@
         <v>2992.3115999999995</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="66">
         <f t="shared" si="1"/>
         <v>5000</v>
@@ -3914,34 +4002,34 @@
   <sheetPr codeName="List4"/>
   <dimension ref="C3:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+    <sheetView topLeftCell="B37" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C3" s="84" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="83"/>
     </row>
-    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3985,7 +4073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -4030,7 +4118,7 @@
         <v>0.24190000000000006</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -4075,7 +4163,7 @@
         <v>2.4207000000000005</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -4120,7 +4208,7 @@
         <v>31.039899999999999</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -4165,7 +4253,7 @@
         <v>344.15880000000004</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -4210,18 +4298,18 @@
         <v>7242.1613999999972</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C13" s="83" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="83"/>
     </row>
-    <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
@@ -4265,7 +4353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C16" s="6">
         <v>100</v>
       </c>
@@ -4310,7 +4398,7 @@
         <v>0.14419999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C17" s="11">
         <v>1000</v>
       </c>
@@ -4355,7 +4443,7 @@
         <v>1.4425000000000003</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C18" s="11">
         <v>10000</v>
       </c>
@@ -4400,7 +4488,7 @@
         <v>18.433799999999998</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C19" s="11">
         <v>100000</v>
       </c>
@@ -4445,7 +4533,7 @@
         <v>206.30410000000001</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C20" s="16">
         <v>1000000</v>
       </c>
@@ -4490,11 +4578,11 @@
         <v>3455.6234999999992</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C23" s="83"/>
       <c r="D23" s="83"/>
     </row>
-    <row r="25" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C25" s="46"/>
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
@@ -4510,7 +4598,7 @@
       <c r="O25" s="47"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C26" s="49"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
@@ -4526,7 +4614,7 @@
       <c r="O26" s="50"/>
       <c r="P26" s="51"/>
     </row>
-    <row r="27" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C27" s="49"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
@@ -4542,7 +4630,7 @@
       <c r="O27" s="47"/>
       <c r="P27" s="51"/>
     </row>
-    <row r="28" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C28" s="49"/>
       <c r="D28" s="47"/>
       <c r="E28" s="47"/>
@@ -4558,7 +4646,7 @@
       <c r="O28" s="47"/>
       <c r="P28" s="51"/>
     </row>
-    <row r="29" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C29" s="49" t="s">
         <v>34</v>
       </c>
@@ -4576,7 +4664,7 @@
       <c r="O29" s="47"/>
       <c r="P29" s="51"/>
     </row>
-    <row r="30" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
@@ -4620,7 +4708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C31" s="6">
         <v>100</v>
       </c>
@@ -4665,7 +4753,7 @@
         <v>0.27639999999999992</v>
       </c>
     </row>
-    <row r="32" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C32" s="11">
         <v>1000</v>
       </c>
@@ -4710,7 +4798,7 @@
         <v>2.8084999999999996</v>
       </c>
     </row>
-    <row r="33" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C33" s="11">
         <v>10000</v>
       </c>
@@ -4755,7 +4843,7 @@
         <v>31.229899999999997</v>
       </c>
     </row>
-    <row r="34" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C34" s="11">
         <v>100000</v>
       </c>
@@ -4800,7 +4888,7 @@
         <v>423.59579999999988</v>
       </c>
     </row>
-    <row r="35" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C35" s="16">
         <v>1000000</v>
       </c>
@@ -4845,8 +4933,8 @@
         <v>8392.0365000000002</v>
       </c>
     </row>
-    <row r="36" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C37" s="71" t="s">
         <v>29</v>
       </c>
@@ -4870,7 +4958,7 @@
       <c r="O37" s="47"/>
       <c r="P37" s="48"/>
     </row>
-    <row r="38" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C38" s="70">
         <f t="shared" ref="C38:C42" si="3">C16</f>
         <v>100</v>
@@ -4898,7 +4986,7 @@
       <c r="O38" s="50"/>
       <c r="P38" s="51"/>
     </row>
-    <row r="39" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C39" s="68">
         <f t="shared" si="3"/>
         <v>1000</v>
@@ -4926,7 +5014,7 @@
       <c r="O39" s="47"/>
       <c r="P39" s="51"/>
     </row>
-    <row r="40" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C40" s="68">
         <f t="shared" si="3"/>
         <v>10000</v>
@@ -4954,7 +5042,7 @@
       <c r="O40" s="47"/>
       <c r="P40" s="51"/>
     </row>
-    <row r="41" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C41" s="68">
         <f t="shared" si="3"/>
         <v>100000</v>
@@ -4982,7 +5070,7 @@
       <c r="O41" s="47"/>
       <c r="P41" s="51"/>
     </row>
-    <row r="42" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C42" s="69">
         <f t="shared" si="3"/>
         <v>1000000</v>
@@ -5030,30 +5118,30 @@
       <selection activeCell="B28" sqref="B28:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -5097,7 +5185,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B10" s="6">
         <v>100</v>
       </c>
@@ -5142,7 +5230,7 @@
         <v>2.0400000000000008E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B11" s="11">
         <v>1000</v>
       </c>
@@ -5187,7 +5275,7 @@
         <v>0.18749999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="11">
         <v>10000</v>
       </c>
@@ -5232,7 +5320,7 @@
         <v>7.5683999999999996</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B13" s="11">
         <v>100000</v>
       </c>
@@ -5277,7 +5365,7 @@
         <v>533.43119999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="16">
         <v>1000000</v>
       </c>
@@ -5322,12 +5410,12 @@
         <v>48808.42779999999</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
@@ -5371,7 +5459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B19" s="6">
         <v>100</v>
       </c>
@@ -5416,7 +5504,7 @@
         <v>0.4210000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B20" s="11">
         <v>1000</v>
       </c>
@@ -5461,7 +5549,7 @@
         <v>2.0110000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>10000</v>
       </c>
@@ -5506,7 +5594,7 @@
         <v>11.015899999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" ht="21" x14ac:dyDescent="0.4">
       <c r="B22" s="11">
         <v>100000</v>
       </c>
@@ -5551,7 +5639,7 @@
         <v>195.0309</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="16">
         <v>1000000</v>
       </c>
@@ -5596,8 +5684,8 @@
         <v>3491.6588999999994</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="63" t="s">
         <v>28</v>
       </c>
@@ -5608,7 +5696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="67">
         <f t="shared" ref="B29:B33" si="2">B10</f>
         <v>100</v>
@@ -5622,7 +5710,7 @@
         <v>0.4210000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="65">
         <f t="shared" si="2"/>
         <v>1000</v>
@@ -5636,7 +5724,7 @@
         <v>2.0110000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="65">
         <f t="shared" si="2"/>
         <v>10000</v>
@@ -5650,7 +5738,7 @@
         <v>11.015899999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="65">
         <f t="shared" si="2"/>
         <v>100000</v>
@@ -5664,7 +5752,7 @@
         <v>195.0309</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="66">
         <f t="shared" si="2"/>
         <v>1000000</v>
@@ -5693,23 +5781,23 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -5756,7 +5844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>5</v>
       </c>
@@ -5805,7 +5893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>10</v>
       </c>
@@ -5854,7 +5942,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>15</v>
       </c>
@@ -5903,7 +5991,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>20</v>
       </c>
@@ -5952,7 +6040,7 @@
         <v>2097151</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>25</v>
       </c>
@@ -6001,8 +6089,8 @@
         <v>67108863</v>
       </c>
     </row>
-    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="63" t="s">
         <v>28</v>
       </c>
@@ -6010,7 +6098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="67">
         <f t="shared" ref="C28:C32" si="2">C6</f>
         <v>5</v>
@@ -6020,7 +6108,7 @@
         <v>0.21230000000000007</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="65">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -6030,7 +6118,7 @@
         <v>1.0325</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="65">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6040,7 +6128,7 @@
         <v>11.912300000000002</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="65">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -6050,7 +6138,7 @@
         <v>690.39210000000003</v>
       </c>
     </row>
-    <row r="32" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="66">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -6075,22 +6163,22 @@
       <selection activeCell="J27" sqref="J27:L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -6134,7 +6222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -6179,7 +6267,7 @@
         <v>0.5615</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -6224,7 +6312,7 @@
         <v>1.3806000000000005</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -6269,7 +6357,7 @@
         <v>4.577</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -6314,7 +6402,7 @@
         <v>36.030700000000003</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -6359,12 +6447,12 @@
         <v>444.37759999999997</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C14" s="46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
@@ -6408,7 +6496,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C16" s="6">
         <v>100</v>
       </c>
@@ -6453,7 +6541,7 @@
         <v>1.1000000000000009E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C17" s="11">
         <v>1000</v>
       </c>
@@ -6498,7 +6586,7 @@
         <v>5.200000000000005E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C18" s="11">
         <v>10000</v>
       </c>
@@ -6543,7 +6631,7 @@
         <v>0.16189999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.4">
       <c r="C19" s="11">
         <v>100000</v>
       </c>
@@ -6588,7 +6676,7 @@
         <v>5.0553000000000008</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C20" s="16">
         <v>1000000</v>
       </c>
@@ -6633,8 +6721,8 @@
         <v>16.159400000000002</v>
       </c>
     </row>
-    <row r="26" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J27" s="63" t="s">
         <v>28</v>
       </c>
@@ -6645,7 +6733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
       <c r="J28" s="67">
         <f t="shared" ref="J28:J32" si="2">C16</f>
         <v>100</v>
@@ -6659,7 +6747,7 @@
         <v>0.5615</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
       <c r="J29" s="65">
         <f t="shared" si="2"/>
         <v>1000</v>
@@ -6673,7 +6761,7 @@
         <v>1.3806000000000005</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
       <c r="J30" s="65">
         <f t="shared" si="2"/>
         <v>10000</v>
@@ -6687,7 +6775,7 @@
         <v>4.577</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="J31" s="65">
         <f t="shared" si="2"/>
         <v>100000</v>
@@ -6701,7 +6789,7 @@
         <v>36.030700000000003</v>
       </c>
     </row>
-    <row r="32" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J32" s="66">
         <f t="shared" si="2"/>
         <v>1000000</v>
@@ -6718,6 +6806,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9D055D-5C66-4AC5-BE40-EFF43743FF28}">
+  <dimension ref="B3:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="88" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="89">
+        <v>125368</v>
+      </c>
+      <c r="C5" s="90">
+        <v>35181</v>
+      </c>
+      <c r="F5" s="85">
+        <v>42</v>
+      </c>
+      <c r="G5" s="92">
+        <v>10</v>
+      </c>
+      <c r="H5" s="92">
+        <v>8</v>
+      </c>
+      <c r="I5" s="92">
+        <v>4</v>
+      </c>
+      <c r="J5" s="92">
+        <v>45</v>
+      </c>
+      <c r="K5" s="92">
+        <v>31</v>
+      </c>
+      <c r="L5" s="86">
+        <f>SUM(F5:K5)</f>
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added statistics for app
</commit_message>
<xml_diff>
--- a/src/main/resources/TESTY.xlsx
+++ b/src/main/resources/TESTY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romis\Documents\Bachelor_thesis_code\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romis\Desktop\fav\Bachelor_thesis_code\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF981668-C1C0-4465-B2D0-AD3CE6C5BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0BEE04-D521-408A-ADA6-6A6BED868D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="7" xr2:uid="{450F20DB-53D6-4CB5-91FD-25E685046F21}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{450F20DB-53D6-4CB5-91FD-25E685046F21}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="53">
   <si>
     <t>Link struktura</t>
   </si>
@@ -211,6 +211,27 @@
   <si>
     <t>Počet testů</t>
   </si>
+  <si>
+    <t>Testy</t>
+  </si>
+  <si>
+    <t>Celkově [Byte]</t>
+  </si>
+  <si>
+    <t>Nástroje [Byte]</t>
+  </si>
+  <si>
+    <t>Celkem</t>
+  </si>
+  <si>
+    <t>Testy %</t>
+  </si>
+  <si>
+    <t>Kod %</t>
+  </si>
+  <si>
+    <t>Kod</t>
+  </si>
 </sst>
 </file>
 
@@ -724,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -946,39 +967,40 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2597,7 +2619,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2920,20 +2942,20 @@
       <selection activeCell="K15" sqref="K15:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="45"/>
     </row>
-    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
@@ -2977,7 +2999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -3022,7 +3044,7 @@
         <v>0.31240999999999997</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -3067,7 +3089,7 @@
         <v>2.0545</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -3112,7 +3134,7 @@
         <v>10.043800000000001</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -3157,7 +3179,7 @@
         <v>67.405900000000003</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -3202,8 +3224,8 @@
         <v>983.47350000000006</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="63" t="str">
         <f t="shared" ref="K15:K20" si="0">C5</f>
         <v>Šířka [-]</v>
@@ -3212,7 +3234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="K16" s="61">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3222,7 +3244,7 @@
         <v>0.31240999999999997</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="K17" s="58">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -3232,7 +3254,7 @@
         <v>2.0545</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="K18" s="58">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -3242,7 +3264,7 @@
         <v>10.043800000000001</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="K19" s="58">
         <f t="shared" si="0"/>
         <v>100000</v>
@@ -3252,7 +3274,7 @@
         <v>67.405900000000003</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K20" s="53">
         <f t="shared" si="0"/>
         <v>1000000</v>
@@ -3262,7 +3284,7 @@
         <v>983.47350000000006</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C27" s="54"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
@@ -3270,7 +3292,7 @@
       <c r="G27" s="55"/>
       <c r="H27" s="55"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C28" s="54"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -3294,17 +3316,17 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3348,7 +3370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -3393,7 +3415,7 @@
         <v>0.20220000000000002</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -3438,7 +3460,7 @@
         <v>0.52510000000000001</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -3483,7 +3505,7 @@
         <v>3.4866000000000001</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -3528,7 +3550,7 @@
         <v>40.417499999999997</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -3573,8 +3595,8 @@
         <v>434.0449999999999</v>
       </c>
     </row>
-    <row r="24" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="63" t="s">
         <v>1</v>
       </c>
@@ -3582,7 +3604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" s="67">
         <f t="shared" ref="D26:D30" si="1">C6</f>
         <v>100</v>
@@ -3592,7 +3614,7 @@
         <v>0.20220000000000002</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="65">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -3602,7 +3624,7 @@
         <v>0.52510000000000001</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" s="65">
         <f t="shared" si="1"/>
         <v>10000</v>
@@ -3612,7 +3634,7 @@
         <v>3.4866000000000001</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" s="65">
         <f t="shared" si="1"/>
         <v>100000</v>
@@ -3622,7 +3644,7 @@
         <v>40.417499999999997</v>
       </c>
     </row>
-    <row r="30" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="66">
         <f t="shared" si="1"/>
         <v>1000000</v>
@@ -3648,22 +3670,22 @@
       <selection activeCell="C28" sqref="C28:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3707,7 +3729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -3752,7 +3774,7 @@
         <v>4.8865999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>500</v>
       </c>
@@ -3797,7 +3819,7 @@
         <v>145.55210000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>1000</v>
       </c>
@@ -3842,7 +3864,7 @@
         <v>710.81810000000007</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>2000</v>
       </c>
@@ -3887,7 +3909,7 @@
         <v>2992.3115999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>5000</v>
       </c>
@@ -3932,8 +3954,8 @@
         <v>21777.465200000002</v>
       </c>
     </row>
-    <row r="27" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="63" t="s">
         <v>28</v>
       </c>
@@ -3941,7 +3963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="67">
         <f t="shared" ref="C29:C33" si="1">C6</f>
         <v>100</v>
@@ -3951,7 +3973,7 @@
         <v>4.8865999999999996</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="65">
         <f t="shared" si="1"/>
         <v>500</v>
@@ -3961,7 +3983,7 @@
         <v>145.55210000000002</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="65">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -3971,7 +3993,7 @@
         <v>710.81810000000007</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="65">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -3981,7 +4003,7 @@
         <v>2992.3115999999995</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="66">
         <f t="shared" si="1"/>
         <v>5000</v>
@@ -4006,30 +4028,30 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C3" s="84" t="s">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="83"/>
-    </row>
-    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="91"/>
+    </row>
+    <row r="4" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
@@ -4073,7 +4095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -4118,7 +4140,7 @@
         <v>0.24190000000000006</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -4163,7 +4185,7 @@
         <v>2.4207000000000005</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -4208,7 +4230,7 @@
         <v>31.039899999999999</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -4253,7 +4275,7 @@
         <v>344.15880000000004</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -4298,18 +4320,18 @@
         <v>7242.1613999999972</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C13" s="83" t="s">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="83"/>
-    </row>
-    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="91"/>
+    </row>
+    <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
@@ -4353,7 +4375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C16" s="6">
         <v>100</v>
       </c>
@@ -4398,7 +4420,7 @@
         <v>0.14419999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C17" s="11">
         <v>1000</v>
       </c>
@@ -4443,7 +4465,7 @@
         <v>1.4425000000000003</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C18" s="11">
         <v>10000</v>
       </c>
@@ -4488,7 +4510,7 @@
         <v>18.433799999999998</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C19" s="11">
         <v>100000</v>
       </c>
@@ -4533,7 +4555,7 @@
         <v>206.30410000000001</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="16">
         <v>1000000</v>
       </c>
@@ -4578,11 +4600,11 @@
         <v>3455.6234999999992</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-    </row>
-    <row r="25" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+    </row>
+    <row r="25" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C25" s="46"/>
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
@@ -4598,7 +4620,7 @@
       <c r="O25" s="47"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C26" s="49"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
@@ -4614,7 +4636,7 @@
       <c r="O26" s="50"/>
       <c r="P26" s="51"/>
     </row>
-    <row r="27" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C27" s="49"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
@@ -4630,7 +4652,7 @@
       <c r="O27" s="47"/>
       <c r="P27" s="51"/>
     </row>
-    <row r="28" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C28" s="49"/>
       <c r="D28" s="47"/>
       <c r="E28" s="47"/>
@@ -4646,7 +4668,7 @@
       <c r="O28" s="47"/>
       <c r="P28" s="51"/>
     </row>
-    <row r="29" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="49" t="s">
         <v>34</v>
       </c>
@@ -4664,7 +4686,7 @@
       <c r="O29" s="47"/>
       <c r="P29" s="51"/>
     </row>
-    <row r="30" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
@@ -4708,7 +4730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C31" s="6">
         <v>100</v>
       </c>
@@ -4753,7 +4775,7 @@
         <v>0.27639999999999992</v>
       </c>
     </row>
-    <row r="32" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C32" s="11">
         <v>1000</v>
       </c>
@@ -4798,7 +4820,7 @@
         <v>2.8084999999999996</v>
       </c>
     </row>
-    <row r="33" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C33" s="11">
         <v>10000</v>
       </c>
@@ -4843,7 +4865,7 @@
         <v>31.229899999999997</v>
       </c>
     </row>
-    <row r="34" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C34" s="11">
         <v>100000</v>
       </c>
@@ -4888,7 +4910,7 @@
         <v>423.59579999999988</v>
       </c>
     </row>
-    <row r="35" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="16">
         <v>1000000</v>
       </c>
@@ -4933,8 +4955,8 @@
         <v>8392.0365000000002</v>
       </c>
     </row>
-    <row r="36" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="71" t="s">
         <v>29</v>
       </c>
@@ -4958,7 +4980,7 @@
       <c r="O37" s="47"/>
       <c r="P37" s="48"/>
     </row>
-    <row r="38" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C38" s="70">
         <f t="shared" ref="C38:C42" si="3">C16</f>
         <v>100</v>
@@ -4986,7 +5008,7 @@
       <c r="O38" s="50"/>
       <c r="P38" s="51"/>
     </row>
-    <row r="39" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C39" s="68">
         <f t="shared" si="3"/>
         <v>1000</v>
@@ -5014,7 +5036,7 @@
       <c r="O39" s="47"/>
       <c r="P39" s="51"/>
     </row>
-    <row r="40" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="40" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C40" s="68">
         <f t="shared" si="3"/>
         <v>10000</v>
@@ -5042,7 +5064,7 @@
       <c r="O40" s="47"/>
       <c r="P40" s="51"/>
     </row>
-    <row r="41" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C41" s="68">
         <f t="shared" si="3"/>
         <v>100000</v>
@@ -5070,7 +5092,7 @@
       <c r="O41" s="47"/>
       <c r="P41" s="51"/>
     </row>
-    <row r="42" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C42" s="69">
         <f t="shared" si="3"/>
         <v>1000000</v>
@@ -5118,30 +5140,30 @@
       <selection activeCell="B28" sqref="B28:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -5185,7 +5207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>100</v>
       </c>
@@ -5230,7 +5252,7 @@
         <v>2.0400000000000008E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="11">
         <v>1000</v>
       </c>
@@ -5275,7 +5297,7 @@
         <v>0.18749999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>10000</v>
       </c>
@@ -5320,7 +5342,7 @@
         <v>7.5683999999999996</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="11">
         <v>100000</v>
       </c>
@@ -5365,7 +5387,7 @@
         <v>533.43119999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="16">
         <v>1000000</v>
       </c>
@@ -5410,12 +5432,12 @@
         <v>48808.42779999999</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
@@ -5459,7 +5481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>100</v>
       </c>
@@ -5504,7 +5526,7 @@
         <v>0.4210000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>1000</v>
       </c>
@@ -5549,7 +5571,7 @@
         <v>2.0110000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B21" s="11">
         <v>10000</v>
       </c>
@@ -5594,7 +5616,7 @@
         <v>11.015899999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>100000</v>
       </c>
@@ -5639,7 +5661,7 @@
         <v>195.0309</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="16">
         <v>1000000</v>
       </c>
@@ -5684,8 +5706,8 @@
         <v>3491.6588999999994</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="63" t="s">
         <v>28</v>
       </c>
@@ -5696,7 +5718,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="67">
         <f t="shared" ref="B29:B33" si="2">B10</f>
         <v>100</v>
@@ -5710,7 +5732,7 @@
         <v>0.4210000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="65">
         <f t="shared" si="2"/>
         <v>1000</v>
@@ -5724,7 +5746,7 @@
         <v>2.0110000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="65">
         <f t="shared" si="2"/>
         <v>10000</v>
@@ -5738,7 +5760,7 @@
         <v>11.015899999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="65">
         <f t="shared" si="2"/>
         <v>100000</v>
@@ -5752,7 +5774,7 @@
         <v>195.0309</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="66">
         <f t="shared" si="2"/>
         <v>1000000</v>
@@ -5781,23 +5803,23 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -5844,7 +5866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>5</v>
       </c>
@@ -5893,7 +5915,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>10</v>
       </c>
@@ -5942,7 +5964,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>15</v>
       </c>
@@ -5991,7 +6013,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>20</v>
       </c>
@@ -6040,7 +6062,7 @@
         <v>2097151</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>25</v>
       </c>
@@ -6089,8 +6111,8 @@
         <v>67108863</v>
       </c>
     </row>
-    <row r="26" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="63" t="s">
         <v>28</v>
       </c>
@@ -6098,7 +6120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="67">
         <f t="shared" ref="C28:C32" si="2">C6</f>
         <v>5</v>
@@ -6108,7 +6130,7 @@
         <v>0.21230000000000007</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="65">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -6118,7 +6140,7 @@
         <v>1.0325</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="65">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6128,7 +6150,7 @@
         <v>11.912300000000002</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="65">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -6138,7 +6160,7 @@
         <v>690.39210000000003</v>
       </c>
     </row>
-    <row r="32" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="66">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -6163,22 +6185,22 @@
       <selection activeCell="J27" sqref="J27:L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -6222,7 +6244,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="6">
         <v>100</v>
       </c>
@@ -6267,7 +6289,7 @@
         <v>0.5615</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="11">
         <v>1000</v>
       </c>
@@ -6312,7 +6334,7 @@
         <v>1.3806000000000005</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C8" s="11">
         <v>10000</v>
       </c>
@@ -6357,7 +6379,7 @@
         <v>4.577</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
         <v>100000</v>
       </c>
@@ -6402,7 +6424,7 @@
         <v>36.030700000000003</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <v>1000000</v>
       </c>
@@ -6447,12 +6469,12 @@
         <v>444.37759999999997</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
@@ -6496,7 +6518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C16" s="6">
         <v>100</v>
       </c>
@@ -6541,7 +6563,7 @@
         <v>1.1000000000000009E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C17" s="11">
         <v>1000</v>
       </c>
@@ -6586,7 +6608,7 @@
         <v>5.200000000000005E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C18" s="11">
         <v>10000</v>
       </c>
@@ -6631,7 +6653,7 @@
         <v>0.16189999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:16" ht="21" x14ac:dyDescent="0.35">
       <c r="C19" s="11">
         <v>100000</v>
       </c>
@@ -6676,7 +6698,7 @@
         <v>5.0553000000000008</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="16">
         <v>1000000</v>
       </c>
@@ -6721,8 +6743,8 @@
         <v>16.159400000000002</v>
       </c>
     </row>
-    <row r="26" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J27" s="63" t="s">
         <v>28</v>
       </c>
@@ -6733,7 +6755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J28" s="67">
         <f t="shared" ref="J28:J32" si="2">C16</f>
         <v>100</v>
@@ -6747,7 +6769,7 @@
         <v>0.5615</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J29" s="65">
         <f t="shared" si="2"/>
         <v>1000</v>
@@ -6761,7 +6783,7 @@
         <v>1.3806000000000005</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J30" s="65">
         <f t="shared" si="2"/>
         <v>10000</v>
@@ -6775,7 +6797,7 @@
         <v>4.577</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J31" s="65">
         <f t="shared" si="2"/>
         <v>100000</v>
@@ -6789,7 +6811,7 @@
         <v>36.030700000000003</v>
       </c>
     </row>
-    <row r="32" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J32" s="66">
         <f t="shared" si="2"/>
         <v>1000000</v>
@@ -6811,83 +6833,154 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9D055D-5C66-4AC5-BE40-EFF43743FF28}">
-  <dimension ref="B3:L5"/>
+  <dimension ref="A3:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="87" t="s">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="91" t="s">
+      <c r="I4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="91" t="s">
+      <c r="J4" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="88" t="s">
+      <c r="L4" s="86" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89">
+      <c r="P4" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="86" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="87">
         <v>125368</v>
       </c>
-      <c r="C5" s="90">
+      <c r="C5" s="88">
         <v>35181</v>
       </c>
-      <c r="F5" s="85">
+      <c r="F5" s="83">
         <v>42</v>
       </c>
-      <c r="G5" s="92">
+      <c r="G5" s="90">
         <v>10</v>
       </c>
-      <c r="H5" s="92">
+      <c r="H5" s="90">
         <v>8</v>
       </c>
-      <c r="I5" s="92">
+      <c r="I5" s="90">
         <v>4</v>
       </c>
-      <c r="J5" s="92">
+      <c r="J5" s="90">
         <v>45</v>
       </c>
-      <c r="K5" s="92">
+      <c r="K5" s="90">
         <v>31</v>
       </c>
-      <c r="L5" s="86">
+      <c r="L5" s="84">
         <f>SUM(F5:K5)</f>
         <v>140</v>
+      </c>
+      <c r="P5" s="83">
+        <v>217731</v>
+      </c>
+      <c r="Q5" s="90">
+        <v>73985</v>
+      </c>
+      <c r="R5" s="84">
+        <v>12419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="93">
+        <f>(B5+C5)</f>
+        <v>160549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <f>B5/B7 * 100</f>
+        <v>78.087063762465036</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8">
+        <f>Q5+R5</f>
+        <v>86404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <f xml:space="preserve"> C5/B7 *100</f>
+        <v>21.912936237534957</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9">
+        <f>R5/R8 *100</f>
+        <v>14.373177167723716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10">
+        <f xml:space="preserve"> Q5/R8 *100</f>
+        <v>85.626822832276289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>